<commit_message>
feat: se añadió flujo de validación y reportes
</commit_message>
<xml_diff>
--- a/documents/reporte.xlsx
+++ b/documents/reporte.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gianp\Documents\Proyectos\UPC\algoritmos-estructuras-datos\PROYECTO_RETC_SIN_DB\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D4C6B4-9738-4457-8CC5-B7B5D995BDA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE80E8F-50A0-4BD6-BB7F-4D57D5E190A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>Codigo Emision</t>
   </si>
@@ -46,6 +46,9 @@
     <t>Cuerpo Receptor</t>
   </si>
   <si>
+    <t>Nombre Cuerpo Receptor</t>
+  </si>
+  <si>
     <t>Cantidad</t>
   </si>
   <si>
@@ -64,9 +67,6 @@
     <t>Local 11 de Empresa 3 SAC</t>
   </si>
   <si>
-    <t>(113,)</t>
-  </si>
-  <si>
     <t>Cultivo de hortalizas y melones, raíces y tubérculos</t>
   </si>
   <si>
@@ -77,6 +77,63 @@
   </si>
   <si>
     <t>ESTIMADO</t>
+  </si>
+  <si>
+    <t>Local 10 de Empresa 3 SAC</t>
+  </si>
+  <si>
+    <t>Xileno</t>
+  </si>
+  <si>
+    <t>Empresa 7 SAC</t>
+  </si>
+  <si>
+    <t>Local 28 de Empresa 7 SAC</t>
+  </si>
+  <si>
+    <t>Cultivo de uva</t>
+  </si>
+  <si>
+    <t>Terreno</t>
+  </si>
+  <si>
+    <t>Tremolita</t>
+  </si>
+  <si>
+    <t>Local 29 de Empresa 7 SAC</t>
+  </si>
+  <si>
+    <t>Zona</t>
+  </si>
+  <si>
+    <t>Uranio</t>
+  </si>
+  <si>
+    <t>MEDIDO</t>
+  </si>
+  <si>
+    <t>Empresa 9 SAC</t>
+  </si>
+  <si>
+    <t>Local 37 de Empresa 9 SAC</t>
+  </si>
+  <si>
+    <t>Silvicultura y otras actividades forestales</t>
+  </si>
+  <si>
+    <t>Agua</t>
+  </si>
+  <si>
+    <t>Triclorobencenos (totales)</t>
+  </si>
+  <si>
+    <t>Empresa 2 SAC</t>
+  </si>
+  <si>
+    <t>Local 6 de Empresa 2 SAC</t>
+  </si>
+  <si>
+    <t>Cultivo de cereales (excepto arroz), legumbres y semillas oleaginosas</t>
   </si>
 </sst>
 </file>
@@ -439,20 +496,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1"/>
-    <col min="7" max="7" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="63.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,8 +556,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
@@ -498,16 +568,16 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
         <v>14</v>
+      </c>
+      <c r="F2">
+        <v>113</v>
       </c>
       <c r="G2" t="s">
         <v>15</v>
@@ -515,13 +585,188 @@
       <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>2.2999999999999998</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>17</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3">
+        <v>113</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3">
+        <v>3.8</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>28</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4">
+        <v>121</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4">
+        <v>12.5</v>
+      </c>
+      <c r="L4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>29</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5">
+        <v>121</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="L5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>37</v>
+      </c>
+      <c r="B6">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6">
+        <v>210</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6">
+        <v>0.75</v>
+      </c>
+      <c r="L6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7">
+        <v>111</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>